<commit_message>
fix, var categories, predict trans cost , update excel file
</commit_message>
<xml_diff>
--- a/public/uploads/expenses_template_TechBudget.xlsx
+++ b/public/uploads/expenses_template_TechBudget.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -31,10 +31,7 @@
     <t xml:space="preserve">description</t>
   </si>
   <si>
-    <t xml:space="preserve">source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cost</t>
+    <t xml:space="preserve">payOption</t>
   </si>
   <si>
     <t xml:space="preserve">category</t>
@@ -49,9 +46,6 @@
     <t xml:space="preserve">Credit</t>
   </si>
   <si>
-    <t xml:space="preserve">Var</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fun</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
     <t xml:space="preserve">Fido</t>
   </si>
   <si>
-    <t xml:space="preserve">Fix</t>
-  </si>
-  <si>
     <t xml:space="preserve">Phone</t>
   </si>
   <si>
@@ -79,6 +70,12 @@
     <t xml:space="preserve">Food</t>
   </si>
   <si>
+    <t xml:space="preserve">STM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dollarama</t>
   </si>
   <si>
@@ -112,10 +109,7 @@
     <t xml:space="preserve">Uber</t>
   </si>
   <si>
-    <t xml:space="preserve">Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UBer</t>
+    <t xml:space="preserve">Maxi</t>
   </si>
   <si>
     <t xml:space="preserve">AWS</t>
@@ -233,23 +227,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -268,340 +263,306 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>11.11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <v>45048</v>
+        <v>45079</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <v>29.62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>45049</v>
+        <v>45080</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>1100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>45050</v>
+        <v>45081</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="0" t="n">
+      <c r="F5" s="0" t="n">
         <v>39.62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>45051</v>
+        <v>45082</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>16.11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>45052</v>
+        <v>45092</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>29.32</v>
+        <v>17</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>35.3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>45053</v>
+        <v>45083</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>31.03</v>
+        <v>20</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>29.32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>45054</v>
+        <v>45084</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>10.9</v>
+        <v>22</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>31.03</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <v>45055</v>
+        <v>45085</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="E10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>9.26</v>
+        <v>8</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>10.9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <v>45056</v>
+        <v>45086</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="E11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>10.9</v>
+        <v>8</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>9.26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <v>45057</v>
+        <v>45087</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>34.5</v>
+      <c r="F12" s="0" t="n">
+        <v>10.9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <v>45058</v>
+        <v>45088</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>7.43</v>
+        <v>15</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>34.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <v>45059</v>
+        <v>45089</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>14.44</v>
+        <v>15</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>7.43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>45060</v>
+        <v>45090</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>13.57</v>
+        <v>17</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>14.44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>45061</v>
+        <v>45091</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>6.9</v>
+        <v>17</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>13.57</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>45062</v>
+        <v>45092</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="0" t="n">
+      <c r="F17" s="0" t="n">
+        <v>44.55</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>45093</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="0" t="n">
         <v>1.58</v>
       </c>
     </row>

</xml_diff>